<commit_message>
Got the items' instances to delete properly after they are used. Changed the rate of gravity so the items dont zoom past the players.
</commit_message>
<xml_diff>
--- a/marioquiz_charts.xlsx
+++ b/marioquiz_charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wandalcooper/Documents/Github_Projects/Games/marioquiz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC3A55CA-BE5A-284F-AD48-A01B807D1E63}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{750F010D-2F86-8E4A-9EA1-51AE5B44F44B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{B759B502-8382-004B-85B5-8C8A273AF423}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>mario</t>
   </si>
@@ -88,6 +88,57 @@
   </si>
   <si>
     <t>BlueCoin</t>
+  </si>
+  <si>
+    <t>QuestionBlock</t>
+  </si>
+  <si>
+    <t>PirahnaPlant</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Purpose of the quiz question</t>
+  </si>
+  <si>
+    <t>Student should translate the word into Japanese</t>
+  </si>
+  <si>
+    <t>random image</t>
+  </si>
+  <si>
+    <t>Student should identify the thing(s) in the image.</t>
+  </si>
+  <si>
+    <t>random, difficult to pronounce English word</t>
+  </si>
+  <si>
+    <t>Student should pronounce the word properly.</t>
+  </si>
+  <si>
+    <t>Student should translate the target sentence into Japanese.</t>
+  </si>
+  <si>
+    <t>random, English target sentence</t>
+  </si>
+  <si>
+    <t>random, present-tense verb</t>
+  </si>
+  <si>
+    <t>random English word</t>
+  </si>
+  <si>
+    <t>randomly mix items on the screen</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>shows "Ask me a question."</t>
+  </si>
+  <si>
+    <t>Student should ask a question in English.</t>
   </si>
 </sst>
 </file>
@@ -123,10 +174,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -468,26 +522,26 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -495,17 +549,17 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -513,37 +567,37 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -552,52 +606,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418628F0-8956-5A45-B957-2190024B7C48}">
-  <dimension ref="A4:A11"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.83203125" customWidth="1"/>
+    <col min="3" max="3" width="59.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added images of the players and items to the excel file.
</commit_message>
<xml_diff>
--- a/marioquiz_charts.xlsx
+++ b/marioquiz_charts.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wandalcooper/Documents/Github_Projects/Games/marioquiz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{750F010D-2F86-8E4A-9EA1-51AE5B44F44B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{64802DD2-D7D7-6B4C-978F-40AB72B31004}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{B759B502-8382-004B-85B5-8C8A273AF423}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{B759B502-8382-004B-85B5-8C8A273AF423}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
-    <sheet name="Items" sheetId="2" r:id="rId2"/>
-    <sheet name="Problems" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Player Images" sheetId="6" r:id="rId2"/>
+    <sheet name="Items" sheetId="2" r:id="rId3"/>
+    <sheet name="Item Images" sheetId="7" r:id="rId4"/>
+    <sheet name="Problems" sheetId="3" r:id="rId5"/>
+    <sheet name="Data" sheetId="4" r:id="rId6"/>
+    <sheet name="Event Booleans" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>mario</t>
   </si>
@@ -139,6 +142,54 @@
   </si>
   <si>
     <t>Student should ask a question in English.</t>
+  </si>
+  <si>
+    <t>Players</t>
+  </si>
+  <si>
+    <t>Yammy</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Problems</t>
+  </si>
+  <si>
+    <t>flag 1</t>
+  </si>
+  <si>
+    <t>flag 2</t>
+  </si>
+  <si>
+    <t>flag 3</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>wave wand</t>
+  </si>
+  <si>
+    <t>transition</t>
+  </si>
+  <si>
+    <t>rotate right</t>
+  </si>
+  <si>
+    <t>rotate left</t>
+  </si>
+  <si>
+    <t>mix</t>
+  </si>
+  <si>
+    <t>show black box</t>
+  </si>
+  <si>
+    <t>show question</t>
   </si>
 </sst>
 </file>
@@ -200,6 +251,1366 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>153280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>112340</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>63499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7456FB34-BF87-7540-98BB-10E2ECC2F018}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="6046080"/>
+          <a:ext cx="1191840" cy="723019"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>670400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>6206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>260900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>122199</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13E6BA11-4CA9-1B43-96E6-19A2D68CC55E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495900" y="5899006"/>
+          <a:ext cx="1241500" cy="928793"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>20670</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>189334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>436670</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F0ADE12-2782-874B-B89E-5654FFF0D0C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20670" y="5878934"/>
+          <a:ext cx="1241500" cy="1134566"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>670400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>134818</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>440820</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>46648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CC3D1B7-44A8-CD46-9110-6F2B75E87495}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495900" y="947618"/>
+          <a:ext cx="595920" cy="521430"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>119008</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>436670</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>30838</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81A42776-E69B-DC4A-98D5-2F9C7217CB77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666250" y="931808"/>
+          <a:ext cx="595920" cy="521430"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>670400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>163868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>211240</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>150188</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D752B942-92F9-4046-8A59-731AF98EDC26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495900" y="5040668"/>
+          <a:ext cx="1191840" cy="595920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>70330</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>144508</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>436670</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>130828</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BDEC5CF-0E75-C147-9A1D-46339B391D6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="70330" y="5021308"/>
+          <a:ext cx="1191840" cy="595920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>670400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>105866</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>589800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>92186</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D7D8535-9582-9D47-B80B-D896C8B9B9A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495900" y="1731466"/>
+          <a:ext cx="744900" cy="595920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>517270</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>89346</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>436670</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>75666</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EF3E9EC-26BA-6745-8794-0077903C6E99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="517270" y="1714946"/>
+          <a:ext cx="744900" cy="595920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>670400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>118330</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>211240</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{217D19D0-6686-D049-B44D-A31A97044A30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495900" y="4182330"/>
+          <a:ext cx="1191840" cy="595920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>70330</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>99680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>436670</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>86000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA078A65-A2F7-A94A-9539-CD7C36365CAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="70330" y="4163680"/>
+          <a:ext cx="1191840" cy="595920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>670400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>151404</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>440820</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38404</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8151839D-2843-3D4B-9307-9699694A9EEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495900" y="2589804"/>
+          <a:ext cx="595920" cy="496600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>134174</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>436670</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>21174</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{331B00CB-E4EA-0540-9F8B-2D6075724F9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666250" y="2572574"/>
+          <a:ext cx="595920" cy="496600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>670400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>163770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>738780</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>75600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Picture 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FABE4E31-CC25-3043-B31E-35B3EDDF889B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495900" y="163770"/>
+          <a:ext cx="893880" cy="521430"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>368290</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>148670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>436670</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>60500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Picture 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6EC48C7-44DC-7C41-9D4C-AC213AB7689E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="368290" y="148670"/>
+          <a:ext cx="893880" cy="521430"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>368290</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>79682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>436670</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>41172</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Picture 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43AE0CA6-9E3B-364D-9D63-D20CBF7079F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="368290" y="3330882"/>
+          <a:ext cx="893880" cy="571090"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>670400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>97622</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>291840</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>59112</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F104FDA9-8F1F-6C4B-B0A7-98416C7A5E26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495900" y="3348822"/>
+          <a:ext cx="446940" cy="571090"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>573900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>37049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>550903</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BA602A2-C7A9-A94A-A4F7-E6CD7440B700}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2224900" y="240249"/>
+          <a:ext cx="802503" cy="432852"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>223119</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>11107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200120</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>35701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D172C8A2-73DC-0B42-8A93-AB58ED3A1C09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1048619" y="214307"/>
+          <a:ext cx="802501" cy="430994"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>249200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>29470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>173000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79AB17E8-0442-3C47-B1D1-4C169357825A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="249200" y="2467870"/>
+          <a:ext cx="581100" cy="549930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>691300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60796</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>737450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>145200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0A14E42-7039-ED43-B0DC-3178E141D93E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3167800" y="2499196"/>
+          <a:ext cx="871650" cy="490804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561900</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C89C296C-A2AB-BB49-B79D-E2BB3D7666D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2212900" y="2495400"/>
+          <a:ext cx="581100" cy="581100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457900</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>54600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>213500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>26100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFC2C236-F88B-8E49-8975-5F5A6DA76E0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1283400" y="2493000"/>
+          <a:ext cx="581100" cy="581100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>573900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>146826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>664500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>198476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B52FD16A-5989-514E-96E5-0008AC030A47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2224900" y="959626"/>
+          <a:ext cx="916100" cy="458050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>109520</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>119026</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200120</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>170676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19029919-EF45-5C47-BE06-E198024673E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="935020" y="931826"/>
+          <a:ext cx="916100" cy="458050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>573900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>78600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>723220</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>31600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{473D78F4-ECE6-8644-B357-43AFB04A1D6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2224900" y="1704200"/>
+          <a:ext cx="1800320" cy="562600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200120</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D1D0A9-B201-9E48-B4CF-A65491AE68A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="50800" y="1676400"/>
+          <a:ext cx="1800320" cy="562600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -605,10 +2016,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF9BC2F-FDD3-D540-9428-E4579983D2C1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418628F0-8956-5A45-B957-2190024B7C48}">
   <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -724,7 +2151,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2F1805-8645-2B4F-9882-D5B1E2E20303}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD9AEB5-832C-9B48-9E49-799254412CE6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -736,7 +2179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7CD25B-3EA9-8D40-AE5A-970F0355FEA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -746,4 +2189,99 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FABB84-A035-794A-81AD-E394D3DE7B5E}">
+  <dimension ref="A2:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Gave the items' problems the added pyglet.text.Label of an English explanation on how to answer the question. Working on how to use Japanese character within pyglet.
</commit_message>
<xml_diff>
--- a/marioquiz_charts.xlsx
+++ b/marioquiz_charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wandalcooper/Documents/Github_Projects/Games/marioquiz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{64802DD2-D7D7-6B4C-978F-40AB72B31004}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{20654FD3-35FD-9841-BD5B-E6184EA7380A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{B759B502-8382-004B-85B5-8C8A273AF423}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="6" xr2:uid="{B759B502-8382-004B-85B5-8C8A273AF423}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="112">
   <si>
     <t>mario</t>
   </si>
@@ -144,59 +144,236 @@
     <t>Student should ask a question in English.</t>
   </si>
   <si>
-    <t>Players</t>
-  </si>
-  <si>
-    <t>Yammy</t>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>Problems</t>
-  </si>
-  <si>
-    <t>flag 1</t>
-  </si>
-  <si>
-    <t>flag 2</t>
-  </si>
-  <si>
-    <t>flag 3</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>wave wand</t>
-  </si>
-  <si>
-    <t>transition</t>
-  </si>
-  <si>
-    <t>rotate right</t>
-  </si>
-  <si>
-    <t>rotate left</t>
-  </si>
-  <si>
-    <t>mix</t>
-  </si>
-  <si>
-    <t>show black box</t>
-  </si>
-  <si>
-    <t>show question</t>
+    <t>objects.Player.randomized</t>
+  </si>
+  <si>
+    <t>default state</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>randomize_players()</t>
+  </si>
+  <si>
+    <t>game.py</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>default state ==&gt;</t>
+  </si>
+  <si>
+    <t>flag ==&gt;</t>
+  </si>
+  <si>
+    <t>on_draw()</t>
+  </si>
+  <si>
+    <t>problems.showing_black_box</t>
+  </si>
+  <si>
+    <t>problems.Problem.vocab_black_box.draw()</t>
+  </si>
+  <si>
+    <t>all_players[0].inventory[0].problem.question.draw()</t>
+  </si>
+  <si>
+    <t>update()</t>
+  </si>
+  <si>
+    <t>items.bombomb_effect</t>
+  </si>
+  <si>
+    <t>mix_items()</t>
+  </si>
+  <si>
+    <t>item_sequence()</t>
+  </si>
+  <si>
+    <t>player.has_item(); len(inventory) &gt; 0</t>
+  </si>
+  <si>
+    <t>FALSE (len = 0)</t>
+  </si>
+  <si>
+    <t>player.use_item()</t>
+  </si>
+  <si>
+    <t>yammy.inventory; len(inventory) &gt; 0</t>
+  </si>
+  <si>
+    <t>yammy.inventory[0].upate()</t>
+  </si>
+  <si>
+    <t>yammy.inventory[0].transition()</t>
+  </si>
+  <si>
+    <t>key.F</t>
+  </si>
+  <si>
+    <t>yammy.transitioning</t>
+  </si>
+  <si>
+    <t>yammy.toggle_transition_direction()</t>
+  </si>
+  <si>
+    <t>player_movement();</t>
+  </si>
+  <si>
+    <t>The conditions on the right must be in the states shown in order to execute the functions on the left.</t>
+  </si>
+  <si>
+    <t>key._1</t>
+  </si>
+  <si>
+    <t>any_movement()</t>
+  </si>
+  <si>
+    <t>yammy.wave_wand()</t>
+  </si>
+  <si>
+    <t>yammy.take_item()</t>
+  </si>
+  <si>
+    <t>new_item()</t>
+  </si>
+  <si>
+    <t>rotate_players_left()</t>
+  </si>
+  <si>
+    <t>rotate_players_right()</t>
+  </si>
+  <si>
+    <t>key.LEFT</t>
+  </si>
+  <si>
+    <t>key.RIGHT</t>
+  </si>
+  <si>
+    <t>key.UP</t>
+  </si>
+  <si>
+    <t>mix_players()</t>
+  </si>
+  <si>
+    <t>key.O</t>
+  </si>
+  <si>
+    <t>right_answer()</t>
+  </si>
+  <si>
+    <t>all_players[0].item</t>
+  </si>
+  <si>
+    <t>key.X</t>
+  </si>
+  <si>
+    <t>item.movement()</t>
+  </si>
+  <si>
+    <t>rotate_items_left()</t>
+  </si>
+  <si>
+    <t>key.A</t>
+  </si>
+  <si>
+    <t>key.D</t>
+  </si>
+  <si>
+    <t>key.S</t>
+  </si>
+  <si>
+    <t>rotate_items_right()</t>
+  </si>
+  <si>
+    <t>objects.py</t>
+  </si>
+  <si>
+    <t>flags</t>
+  </si>
+  <si>
+    <t>"walk"</t>
+  </si>
+  <si>
+    <t>Player.randomized</t>
+  </si>
+  <si>
+    <t>Player.game_just_started</t>
+  </si>
+  <si>
+    <t>Player.debug</t>
+  </si>
+  <si>
+    <t>Player.__init__.item</t>
+  </si>
+  <si>
+    <t>Player.__init__.speed</t>
+  </si>
+  <si>
+    <t>Player.__init__.moving</t>
+  </si>
+  <si>
+    <t>Player.__init__.rotating_players</t>
+  </si>
+  <si>
+    <t>Player.use_item()</t>
+  </si>
+  <si>
+    <t>item.effect()</t>
+  </si>
+  <si>
+    <t>item.item_not_used</t>
+  </si>
+  <si>
+    <t>items.py</t>
+  </si>
+  <si>
+    <t>Item.__init__.transition_direction</t>
+  </si>
+  <si>
+    <t>"out"</t>
+  </si>
+  <si>
+    <t>Item.__init__.moving</t>
+  </si>
+  <si>
+    <t>Item.__init__.falling</t>
+  </si>
+  <si>
+    <t>Item.__init__.transitioning</t>
+  </si>
+  <si>
+    <t>Item.__init__.special</t>
+  </si>
+  <si>
+    <t>Item.__init__.item_not_used</t>
+  </si>
+  <si>
+    <t>util.falling_object()</t>
+  </si>
+  <si>
+    <t>items.Item.__init__.falling</t>
+  </si>
+  <si>
+    <t>problems.py</t>
+  </si>
+  <si>
+    <t>showing_black_box</t>
+  </si>
+  <si>
+    <t>util.py</t>
+  </si>
+  <si>
+    <t>Line.mixing_player_spots</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,13 +381,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -225,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -235,6 +437,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2155,7 +2379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2F1805-8645-2B4F-9882-D5B1E2E20303}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2193,92 +2417,705 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FABB84-A035-794A-81AD-E394D3DE7B5E}">
-  <dimension ref="A2:E20"/>
+  <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1"/>
+    <col min="15" max="15" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="21" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="64" x14ac:dyDescent="0.2">
+      <c r="C4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" t="b">
+        <v>0</v>
+      </c>
+      <c r="P17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B18" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B20" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+      <c r="S22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B24" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="U24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="U25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B26" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="V26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B27" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="N27" t="b">
+        <v>0</v>
+      </c>
+      <c r="W27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B28" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="N28" t="b">
+        <v>0</v>
+      </c>
+      <c r="X28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B32" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B35" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B39" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>52</v>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
game.py: cleaned up the main file by moving player creation code to playersetup.py and by moving game constants to constants.py.
</commit_message>
<xml_diff>
--- a/marioquiz_charts.xlsx
+++ b/marioquiz_charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wandalcooper/Documents/Github_Projects/Games/marioquiz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{20654FD3-35FD-9841-BD5B-E6184EA7380A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{80093B2E-C8FC-1F43-8357-9DB230906A6E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="6" xr2:uid="{B759B502-8382-004B-85B5-8C8A273AF423}"/>
   </bookViews>
@@ -2420,7 +2420,7 @@
   <dimension ref="A1:Y65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>